<commit_message>
Added the core volume to the excel and code
Core volume determines the size therefore I believe it ti also important
</commit_message>
<xml_diff>
--- a/Week2-Assignments/Hakan Polat/Datasheet.xlsx
+++ b/Week2-Assignments/Hakan Polat/Datasheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>N1</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Cost</t>
+  </si>
+  <si>
+    <t>Corevolume</t>
   </si>
 </sst>
 </file>
@@ -391,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L61"/>
+  <dimension ref="A1:M61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -402,9 +405,10 @@
     <col min="3" max="4" width="11.109375" customWidth="1"/>
     <col min="5" max="5" width="11.44140625" customWidth="1"/>
     <col min="6" max="6" width="11.5546875" customWidth="1"/>
+    <col min="13" max="13" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,8 +445,11 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>86</v>
       </c>
@@ -479,8 +486,11 @@
       <c r="L2">
         <v>304706.36388840101</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M2">
+        <v>12.930893025841099</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>173</v>
       </c>
@@ -517,8 +527,11 @@
       <c r="L3">
         <v>157645.94708085601</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M3">
+        <v>6.68304685801668</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>259</v>
       </c>
@@ -555,8 +568,11 @@
       <c r="L4">
         <v>121036.16260945</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4">
+        <v>5.12599848576673</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>345</v>
       </c>
@@ -593,8 +609,11 @@
       <c r="L5">
         <v>105733.497591194</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5">
+        <v>4.4740996614771698</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>431</v>
       </c>
@@ -631,8 +650,11 @@
       <c r="L6">
         <v>97684.059958266895</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M6">
+        <v>4.1304418589971599</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>518</v>
       </c>
@@ -669,8 +691,11 @@
       <c r="L7">
         <v>92852.469250634895</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M7">
+        <v>3.9235999301504698</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>604</v>
       </c>
@@ -707,8 +732,11 @@
       <c r="L8">
         <v>89691.777460558194</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M8">
+        <v>3.78784223347576</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>690</v>
       </c>
@@ -745,8 +773,11 @@
       <c r="L9">
         <v>87494.952333663401</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M9">
+        <v>3.6931188904991301</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>776</v>
       </c>
@@ -783,8 +814,11 @@
       <c r="L10">
         <v>85897.799533261699</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M10">
+        <v>3.6239458311972101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>863</v>
       </c>
@@ -821,8 +855,11 @@
       <c r="L11">
         <v>84695.624846637598</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M11">
+        <v>3.5716175092284801</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>86</v>
       </c>
@@ -859,8 +896,11 @@
       <c r="L12">
         <v>261028.05863513399</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M12">
+        <v>11.0765504046645</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>173</v>
       </c>
@@ -897,8 +937,11 @@
       <c r="L13">
         <v>133565.054290259</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M13">
+        <v>5.6610162370444801</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>259</v>
       </c>
@@ -935,8 +978,11 @@
       <c r="L14">
         <v>101837.379591782</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M14">
+        <v>4.3113913528753303</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>345</v>
       </c>
@@ -973,8 +1019,11 @@
       <c r="L15">
         <v>88577.585471522703</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M15">
+        <v>3.7463357702087099</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>431</v>
       </c>
@@ -1011,8 +1060,11 @@
       <c r="L16">
         <v>81604.267090943205</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M16">
+        <v>3.4484586264204902</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>518</v>
       </c>
@@ -1049,8 +1101,11 @@
       <c r="L17">
         <v>77419.766195012897</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M17">
+        <v>3.2691713163816498</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>604</v>
       </c>
@@ -1087,8 +1142,11 @@
       <c r="L18">
         <v>74683.302436734099</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M18">
+        <v>3.1514986936712099</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>690</v>
       </c>
@@ -1125,8 +1183,11 @@
       <c r="L19">
         <v>72782.087011710202</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M19">
+        <v>3.06939399925621</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>776</v>
       </c>
@@ -1163,8 +1224,11 @@
       <c r="L20">
         <v>71400.481516434404</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M20">
+        <v>3.0094358863216302</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>863</v>
       </c>
@@ -1201,8 +1265,11 @@
       <c r="L21">
         <v>70361.0879878915</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M21">
+        <v>2.9640785250896502</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>86</v>
       </c>
@@ -1239,8 +1306,11 @@
       <c r="L22">
         <v>226728.02799590401</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M22">
+        <v>9.6203896927708303</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>173</v>
       </c>
@@ -1277,8 +1347,11 @@
       <c r="L23">
         <v>114867.031010946</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M23">
+        <v>4.8674920789657996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>259</v>
       </c>
@@ -1315,8 +1388,11 @@
       <c r="L24">
         <v>87025.990817194906</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M24">
+        <v>3.6830052503435802</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>345</v>
       </c>
@@ -1353,8 +1429,11 @@
       <c r="L25">
         <v>75392.433074469402</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M25">
+        <v>3.1870890124623599</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>431</v>
       </c>
@@ -1391,8 +1470,11 @@
       <c r="L26">
         <v>69275.702502718093</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M26">
+        <v>2.9256596645721298</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>518</v>
       </c>
@@ -1429,8 +1511,11 @@
       <c r="L27">
         <v>65606.236830338996</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M27">
+        <v>2.7683096780899001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>604</v>
       </c>
@@ -1467,8 +1552,11 @@
       <c r="L28">
         <v>63207.390314719203</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M28">
+        <v>2.6650352991681099</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>690</v>
       </c>
@@ -1505,8 +1593,11 @@
       <c r="L29">
         <v>61541.402811357999</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M29">
+        <v>2.5929768107367299</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>776</v>
       </c>
@@ -1543,8 +1634,11 @@
       <c r="L30">
         <v>60331.291605460297</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M30">
+        <v>2.5403550816376899</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>863</v>
       </c>
@@ -1581,8 +1675,11 @@
       <c r="L31">
         <v>59421.389212487098</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M31">
+        <v>2.5005475783895501</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>86</v>
       </c>
@@ -1619,8 +1716,11 @@
       <c r="L32">
         <v>199230.900616928</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M32">
+        <v>8.4530623854175495</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>173</v>
       </c>
@@ -1657,8 +1757,11 @@
       <c r="L33">
         <v>100030.621638768</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M33">
+        <v>4.2378903970428796</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>259</v>
       </c>
@@ -1695,8 +1798,11 @@
       <c r="L34">
         <v>75343.394735835696</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M34">
+        <v>3.18741211909613</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>345</v>
       </c>
@@ -1733,8 +1839,11 @@
       <c r="L35">
         <v>65029.376932086103</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M35">
+        <v>2.7476020486192301</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>431</v>
       </c>
@@ -1771,8 +1880,11 @@
       <c r="L36">
         <v>59607.637863125397</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M36">
+        <v>2.5157498704942101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>518</v>
       </c>
@@ -1809,8 +1921,11 @@
       <c r="L37">
         <v>56356.007764692098</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M37">
+        <v>2.3762018917065699</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>604</v>
       </c>
@@ -1847,8 +1962,11 @@
       <c r="L38">
         <v>54231.032199385401</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M38">
+        <v>2.2846116020517999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>690</v>
       </c>
@@ -1885,8 +2003,11 @@
       <c r="L39">
         <v>52755.834481456797</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M39">
+        <v>2.2207055500723998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>776</v>
       </c>
@@ -1923,8 +2044,11 @@
       <c r="L40">
         <v>51684.799449077502</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M40">
+        <v>2.17403725285644</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>863</v>
       </c>
@@ -1961,8 +2085,11 @@
       <c r="L41">
         <v>50879.892841161098</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M41">
+        <v>2.1387334263798601</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>86</v>
       </c>
@@ -1999,8 +2126,11 @@
       <c r="L42">
         <v>176800.35243297499</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M42">
+        <v>7.5008459963847702</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>173</v>
       </c>
@@ -2037,8 +2167,11 @@
       <c r="L43">
         <v>88041.183602678793</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M43">
+        <v>3.72913615950903</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>259</v>
       </c>
@@ -2075,8 +2208,11 @@
       <c r="L44">
         <v>65954.767395788105</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M44">
+        <v>2.7891746904910599</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>345</v>
       </c>
@@ -2113,8 +2249,11 @@
       <c r="L45">
         <v>56728.857321679003</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M45">
+        <v>2.3956353583476102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>431</v>
       </c>
@@ -2151,8 +2290,11 @@
       <c r="L46">
         <v>51880.174941324804</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M46">
+        <v>2.1881754626785801</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>518</v>
       </c>
@@ -2189,8 +2331,11 @@
       <c r="L47">
         <v>48973.040990354602</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M47">
+        <v>2.06330879394927</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>604</v>
       </c>
@@ -2227,8 +2372,11 @@
       <c r="L48">
         <v>47073.841425215403</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M48">
+        <v>1.98135436898015</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>690</v>
       </c>
@@ -2265,8 +2413,11 @@
       <c r="L49">
         <v>45755.9086014118</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M49">
+        <v>1.9241716287381401</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>776</v>
       </c>
@@ -2303,8 +2454,11 @@
       <c r="L50">
         <v>44799.4950889752</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M50">
+        <v>1.88241312489414</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>863</v>
       </c>
@@ -2341,8 +2495,11 @@
       <c r="L51">
         <v>44081.107973193</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M51">
+        <v>1.85082347921223</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>86</v>
       </c>
@@ -2379,8 +2536,11 @@
       <c r="L52">
         <v>158228.56607937001</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M52">
+        <v>6.7124583287213397</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>173</v>
       </c>
@@ -2417,8 +2577,11 @@
       <c r="L53">
         <v>78199.869935009498</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M53">
+        <v>3.3115616392606699</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>259</v>
       </c>
@@ -2455,8 +2618,11 @@
       <c r="L54">
         <v>58288.078078302198</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M54">
+        <v>2.46401185773989</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>345</v>
       </c>
@@ -2493,8 +2659,11 @@
       <c r="L55">
         <v>49971.922042434402</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M55">
+        <v>2.1091630836444102</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>431</v>
       </c>
@@ -2531,8 +2700,11 @@
       <c r="L56">
         <v>45602.331105309197</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M56">
+        <v>1.9220994698217</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>518</v>
       </c>
@@ -2569,8 +2741,11 @@
       <c r="L57">
         <v>42983.179624763499</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M57">
+        <v>1.8095089846911501</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>604</v>
       </c>
@@ -2607,8 +2782,11 @@
       <c r="L58">
         <v>41272.6976074751</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M58">
+        <v>1.7356118545781301</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>690</v>
       </c>
@@ -2645,8 +2823,11 @@
       <c r="L59">
         <v>40086.199810710699</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M59">
+        <v>1.6840509974618201</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>776</v>
       </c>
@@ -2683,8 +2864,11 @@
       <c r="L60">
         <v>39225.567922065202</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M60">
+        <v>1.6463979531869399</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>863</v>
       </c>
@@ -2720,6 +2904,9 @@
       </c>
       <c r="L61">
         <v>38579.4675343661</v>
+      </c>
+      <c r="M61">
+        <v>1.6179140225381701</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Transformer has been selected
I selected the transformer and colored it to yellow on the xlsx sheet. I took cost size and efficiency into consideration
</commit_message>
<xml_diff>
--- a/Week2-Assignments/Hakan Polat/Datasheet.xlsx
+++ b/Week2-Assignments/Hakan Polat/Datasheet.xlsx
@@ -68,12 +68,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -88,8 +94,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,7 +404,7 @@
   <dimension ref="A1:M61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2869,43 +2876,43 @@
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A61">
+      <c r="A61" s="1">
         <v>863</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="1">
         <v>10</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="1">
         <v>1.5</v>
       </c>
-      <c r="D61">
+      <c r="D61" s="1">
         <v>12700.6250769247</v>
       </c>
-      <c r="E61">
+      <c r="E61" s="1">
         <v>47.759230359216502</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="1">
         <v>2.8863967403666102</v>
       </c>
-      <c r="G61">
+      <c r="G61" s="1">
         <v>4.1207269216264998E-4</v>
       </c>
-      <c r="H61">
+      <c r="H61" s="1">
         <v>9.2911041113280604</v>
       </c>
-      <c r="I61">
+      <c r="I61" s="1">
         <v>31751.562692311702</v>
       </c>
-      <c r="J61">
+      <c r="J61" s="1">
         <v>4997.6791537539302</v>
       </c>
-      <c r="K61">
+      <c r="K61" s="1">
         <v>96.455339404866194</v>
       </c>
-      <c r="L61">
+      <c r="L61" s="1">
         <v>38579.4675343661</v>
       </c>
-      <c r="M61">
+      <c r="M61" s="1">
         <v>1.6179140225381701</v>
       </c>
     </row>

</xml_diff>